<commit_message>
add order to ASC and UHC_SM as well as UHC pillar
</commit_message>
<xml_diff>
--- a/data-raw/indicator_df.xlsx
+++ b/data-raw/indicator_df.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ellio\Documents\WHO\billionaiRe\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{406C9BBF-CC22-4964-B938-974A5795BFC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EF5D77E-1965-4558-AF1D-9C5B37DB941A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="32280" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="971" uniqueCount="558">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="973" uniqueCount="558">
   <si>
     <t>dashboard_id</t>
   </si>
@@ -2094,10 +2094,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:Q120"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="Q78" sqref="Q78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2215,7 +2216,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>467</v>
       </c>
@@ -2238,7 +2239,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>372</v>
       </c>
@@ -2285,7 +2286,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>469</v>
       </c>
@@ -2311,7 +2312,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>371</v>
       </c>
@@ -2337,7 +2338,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
         <v>472</v>
       </c>
@@ -2357,7 +2358,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
         <v>473</v>
       </c>
@@ -2377,7 +2378,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
         <v>474</v>
       </c>
@@ -2397,7 +2398,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
         <v>475</v>
       </c>
@@ -2417,7 +2418,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>378</v>
       </c>
@@ -2467,7 +2468,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>392</v>
       </c>
@@ -2517,7 +2518,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
         <v>476</v>
       </c>
@@ -2537,7 +2538,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
         <v>477</v>
       </c>
@@ -2557,7 +2558,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
         <v>478</v>
       </c>
@@ -2577,7 +2578,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
         <v>479</v>
       </c>
@@ -2597,7 +2598,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>274</v>
       </c>
@@ -2650,7 +2651,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
         <v>399</v>
       </c>
@@ -2688,7 +2689,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
         <v>403</v>
       </c>
@@ -2726,7 +2727,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
         <v>407</v>
       </c>
@@ -2764,7 +2765,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>280</v>
       </c>
@@ -2817,7 +2818,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="B22" t="s">
         <v>411</v>
       </c>
@@ -2855,7 +2856,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="B23" t="s">
         <v>415</v>
       </c>
@@ -2896,7 +2897,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>286</v>
       </c>
@@ -2949,7 +2950,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>292</v>
       </c>
@@ -3002,7 +3003,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>297</v>
       </c>
@@ -3055,7 +3056,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="B27" t="s">
         <v>418</v>
       </c>
@@ -3093,7 +3094,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="B28" t="s">
         <v>421</v>
       </c>
@@ -3131,7 +3132,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="B29" t="s">
         <v>425</v>
       </c>
@@ -3169,7 +3170,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>302</v>
       </c>
@@ -3222,7 +3223,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="B31" t="s">
         <v>429</v>
       </c>
@@ -3260,7 +3261,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="B32" t="s">
         <v>433</v>
       </c>
@@ -3298,7 +3299,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>307</v>
       </c>
@@ -3351,7 +3352,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>312</v>
       </c>
@@ -3404,7 +3405,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="B35" t="s">
         <v>437</v>
       </c>
@@ -3442,7 +3443,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="B36" t="s">
         <v>441</v>
       </c>
@@ -3480,7 +3481,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>312</v>
       </c>
@@ -3521,7 +3522,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>317</v>
       </c>
@@ -3574,7 +3575,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="B39" t="s">
         <v>447</v>
       </c>
@@ -3612,7 +3613,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="B40" t="s">
         <v>451</v>
       </c>
@@ -3650,7 +3651,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="B41" t="s">
         <v>455</v>
       </c>
@@ -3688,7 +3689,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>322</v>
       </c>
@@ -3741,7 +3742,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>328</v>
       </c>
@@ -3794,7 +3795,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="44" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="B44" t="s">
         <v>459</v>
       </c>
@@ -3832,7 +3833,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="45" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="B45" t="s">
         <v>463</v>
       </c>
@@ -3870,7 +3871,7 @@
         <v>466</v>
       </c>
     </row>
-    <row r="46" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>333</v>
       </c>
@@ -3923,7 +3924,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="47" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>338</v>
       </c>
@@ -3976,7 +3977,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="48" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>395</v>
       </c>
@@ -4023,7 +4024,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="49" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>480</v>
       </c>
@@ -4046,7 +4047,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="B50" t="s">
         <v>482</v>
       </c>
@@ -4078,7 +4079,7 @@
         <v>518</v>
       </c>
     </row>
-    <row r="51" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="B51" t="s">
         <v>483</v>
       </c>
@@ -4110,7 +4111,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="52" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="B52" t="s">
         <v>484</v>
       </c>
@@ -4142,7 +4143,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="53" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="B53" t="s">
         <v>485</v>
       </c>
@@ -4174,7 +4175,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="54" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>349</v>
       </c>
@@ -4227,7 +4228,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="55" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="B55" t="s">
         <v>486</v>
       </c>
@@ -4259,7 +4260,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="56" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="B56" t="s">
         <v>487</v>
       </c>
@@ -4291,7 +4292,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="57" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="B57" t="s">
         <v>368</v>
       </c>
@@ -4338,7 +4339,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="58" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>488</v>
       </c>
@@ -4376,7 +4377,7 @@
         <v>533</v>
       </c>
     </row>
-    <row r="59" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>367</v>
       </c>
@@ -4414,7 +4415,7 @@
         <v>534</v>
       </c>
     </row>
-    <row r="60" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>363</v>
       </c>
@@ -4464,7 +4465,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="61" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="B61" t="s">
         <v>491</v>
       </c>
@@ -4496,7 +4497,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="62" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>384</v>
       </c>
@@ -4546,7 +4547,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="63" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="B63" t="s">
         <v>492</v>
       </c>
@@ -4578,7 +4579,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="64" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>343</v>
       </c>
@@ -4631,7 +4632,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="65" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="B65" t="s">
         <v>493</v>
       </c>
@@ -4663,7 +4664,7 @@
         <v>537</v>
       </c>
     </row>
-    <row r="66" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>375</v>
       </c>
@@ -4710,7 +4711,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="67" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>388</v>
       </c>
@@ -4760,7 +4761,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="68" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>494</v>
       </c>
@@ -4798,7 +4799,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="69" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="B69" t="s">
         <v>496</v>
       </c>
@@ -4830,7 +4831,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="70" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="B70" t="s">
         <v>360</v>
       </c>
@@ -4877,7 +4878,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="71" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>497</v>
       </c>
@@ -4915,7 +4916,7 @@
         <v>544</v>
       </c>
     </row>
-    <row r="72" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>359</v>
       </c>
@@ -4953,7 +4954,7 @@
         <v>545</v>
       </c>
     </row>
-    <row r="73" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>355</v>
       </c>
@@ -5003,7 +5004,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="74" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="B74" t="s">
         <v>500</v>
       </c>
@@ -5172,6 +5173,12 @@
       <c r="N77" t="s">
         <v>550</v>
       </c>
+      <c r="P77">
+        <v>65</v>
+      </c>
+      <c r="Q77" t="s">
+        <v>513</v>
+      </c>
     </row>
     <row r="78" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
@@ -5916,6 +5923,12 @@
       <c r="O92" t="s">
         <v>551</v>
       </c>
+      <c r="P92">
+        <v>66</v>
+      </c>
+      <c r="Q92" t="s">
+        <v>513</v>
+      </c>
     </row>
     <row r="93" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
@@ -5970,7 +5983,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="94" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>143</v>
       </c>
@@ -6023,7 +6036,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="95" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>121</v>
       </c>
@@ -6076,7 +6089,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="96" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
         <v>48</v>
       </c>
@@ -6129,7 +6142,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="97" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>63</v>
       </c>
@@ -6182,7 +6195,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="98" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>41</v>
       </c>
@@ -6235,7 +6248,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="99" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>114</v>
       </c>
@@ -6288,7 +6301,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="100" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
         <v>514</v>
       </c>
@@ -6317,7 +6330,7 @@
         <v>556</v>
       </c>
     </row>
-    <row r="101" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
         <v>515</v>
       </c>
@@ -6346,7 +6359,7 @@
         <v>557</v>
       </c>
     </row>
-    <row r="102" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
         <v>516</v>
       </c>
@@ -6375,7 +6388,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="103" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="B103" t="s">
         <v>504</v>
       </c>
@@ -6401,7 +6414,7 @@
         <v>555</v>
       </c>
     </row>
-    <row r="104" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
         <v>517</v>
       </c>
@@ -6430,7 +6443,7 @@
         <v>552</v>
       </c>
     </row>
-    <row r="105" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="B105" t="s">
         <v>506</v>
       </c>
@@ -6456,7 +6469,7 @@
         <v>553</v>
       </c>
     </row>
-    <row r="106" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
         <v>99</v>
       </c>
@@ -6509,7 +6522,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="107" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="B107" t="s">
         <v>110</v>
       </c>
@@ -6559,7 +6572,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="108" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="B108" t="s">
         <v>106</v>
       </c>
@@ -6609,7 +6622,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="109" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
         <v>137</v>
       </c>
@@ -6662,7 +6675,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="110" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
         <v>56</v>
       </c>
@@ -6715,7 +6728,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="111" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
         <v>34</v>
       </c>
@@ -6768,7 +6781,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="112" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
         <v>129</v>
       </c>
@@ -6821,7 +6834,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="113" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
         <v>77</v>
       </c>
@@ -6874,7 +6887,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="114" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
         <v>17</v>
       </c>
@@ -6927,7 +6940,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="115" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
         <v>70</v>
       </c>
@@ -6980,7 +6993,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="116" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
         <v>150</v>
       </c>
@@ -7033,7 +7046,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="117" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
         <v>27</v>
       </c>
@@ -7086,7 +7099,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="118" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
         <v>85</v>
       </c>
@@ -7139,7 +7152,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="119" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="B119" t="s">
         <v>96</v>
       </c>
@@ -7189,7 +7202,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="120" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:17" hidden="1" x14ac:dyDescent="0.3">
       <c r="B120" t="s">
         <v>92</v>
       </c>
@@ -7240,7 +7253,13 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:Q120" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:Q120" xr:uid="{00000000-0001-0000-0000-000000000000}">
+    <filterColumn colId="4">
+      <filters>
+        <filter val="TRUE"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:Q120">
     <sortCondition descending="1" ref="G2:G120"/>
     <sortCondition descending="1" ref="E2:E120"/>

</xml_diff>